<commit_message>
Tracabilité des exigences #PrettyColorsAndStuff
</commit_message>
<xml_diff>
--- a/Documentations/Traçabilité des exigences.xlsx
+++ b/Documentations/Traçabilité des exigences.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lavalvirtualworkspace\lv2\Laval-Virtual-2014\Documentations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10488"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="11" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="105">
   <si>
     <t>No. Réf.</t>
   </si>
@@ -183,13 +188,166 @@
   </si>
   <si>
     <t>Implémentée</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>Choix du mode de jeu</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>Mode libre</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>Mode assisté</t>
+  </si>
+  <si>
+    <t>3.1.4</t>
+  </si>
+  <si>
+    <t>Mode néophyte</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Contrôles du présentateur</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>Détection du geste correspondant à chaque instrument</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>Guidage pour le choix de l'instrument</t>
+  </si>
+  <si>
+    <t>3.3.</t>
+  </si>
+  <si>
+    <t>Emplacement de l'instrument</t>
+  </si>
+  <si>
+    <t>3.4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4.4 </t>
+  </si>
+  <si>
+    <t>3.4.5</t>
+  </si>
+  <si>
+    <t>Vue à la première personne (piano)</t>
+  </si>
+  <si>
+    <t>Positionnement du capteur (piano)</t>
+  </si>
+  <si>
+    <t>Notes jouables (piano)</t>
+  </si>
+  <si>
+    <t>Grosseur relative des modèles (piano)</t>
+  </si>
+  <si>
+    <t>Utilisation des pédales (piano)</t>
+  </si>
+  <si>
+    <t>Vue à la première personne (batterie)</t>
+  </si>
+  <si>
+    <t>Positionnement du capteur (batterie)</t>
+  </si>
+  <si>
+    <t>3.5.4</t>
+  </si>
+  <si>
+    <t>Pédale de la batterie (batterie)</t>
+  </si>
+  <si>
+    <t>Jouabilité de la batterie (batterie)</t>
+  </si>
+  <si>
+    <t>Jouabilité de la guitare (guitare)</t>
+  </si>
+  <si>
+    <t>Vue à la troisième personne (guitare)</t>
+  </si>
+  <si>
+    <t>3.6.3</t>
+  </si>
+  <si>
+    <t>Positionnement de capteur (guitare)</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>Instruments souhaitables</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>Instruments optionnels</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>Affichage des instruments de chaque joueur sur un même écran</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>Affichage évolué</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>Nombre de joueurs</t>
+  </si>
+  <si>
+    <t>3.11.1</t>
+  </si>
+  <si>
+    <t>Deux pianos simultanés</t>
+  </si>
+  <si>
+    <t>Non implémenté</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>Implémenté</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>High-hat peu fonctionnel, changement d'algorithme nécéssaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,16 +355,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -227,11 +434,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -260,8 +486,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,7 +774,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,11 +784,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="121.88671875" customWidth="1"/>
   </cols>
@@ -594,19 +836,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8"/>
+    <col min="5" max="5" width="20.88671875" style="8" customWidth="1"/>
     <col min="6" max="6" width="53.88671875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -628,6 +870,373 @@
       </c>
       <c r="F1" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +1253,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
@@ -654,7 +1263,7 @@
     <col min="6" max="6" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>